<commit_message>
feat:"exclusão das pastas e alterações dos nomes"
</commit_message>
<xml_diff>
--- a/relatorio.xlsx
+++ b/relatorio.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E17"/>
+  <dimension ref="A1:E129"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -463,14 +463,14 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>2025-12-15 22:04:54</t>
+          <t>2025-12-17 23:16:31</t>
         </is>
       </c>
       <c r="B2" t="n">
         <v>0</v>
       </c>
       <c r="C2" t="n">
-        <v>50.29</v>
+        <v>45.41</v>
       </c>
       <c r="D2" t="n">
         <v>1.24</v>
@@ -482,14 +482,14 @@
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>2025-12-15 22:04:56</t>
+          <t>2025-12-17 23:16:33</t>
         </is>
       </c>
       <c r="B3" t="n">
-        <v>0</v>
+        <v>2.5</v>
       </c>
       <c r="C3" t="n">
-        <v>50.29</v>
+        <v>45.41</v>
       </c>
       <c r="D3" t="n">
         <v>1.24</v>
@@ -501,14 +501,14 @@
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>2025-12-15 22:04:57</t>
+          <t>2025-12-17 23:16:34</t>
         </is>
       </c>
       <c r="B4" t="n">
-        <v>0</v>
+        <v>27.5</v>
       </c>
       <c r="C4" t="n">
-        <v>50.29</v>
+        <v>45.41</v>
       </c>
       <c r="D4" t="n">
         <v>1.24</v>
@@ -520,14 +520,14 @@
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>2025-12-15 22:04:59</t>
+          <t>2025-12-17 23:16:36</t>
         </is>
       </c>
       <c r="B5" t="n">
-        <v>0</v>
+        <v>27.5</v>
       </c>
       <c r="C5" t="n">
-        <v>50.29</v>
+        <v>45.41</v>
       </c>
       <c r="D5" t="n">
         <v>1.24</v>
@@ -539,14 +539,14 @@
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>2025-12-15 22:05:00</t>
+          <t>2025-12-17 23:16:37</t>
         </is>
       </c>
       <c r="B6" t="n">
-        <v>0</v>
+        <v>27.5</v>
       </c>
       <c r="C6" t="n">
-        <v>50.29</v>
+        <v>45.41</v>
       </c>
       <c r="D6" t="n">
         <v>1.24</v>
@@ -558,14 +558,14 @@
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>2025-12-15 22:05:02</t>
+          <t>2025-12-17 23:16:39</t>
         </is>
       </c>
       <c r="B7" t="n">
-        <v>0</v>
+        <v>27.5</v>
       </c>
       <c r="C7" t="n">
-        <v>50.29</v>
+        <v>45.41</v>
       </c>
       <c r="D7" t="n">
         <v>1.24</v>
@@ -577,14 +577,14 @@
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>2025-12-15 22:05:03</t>
+          <t>2025-12-17 23:16:40</t>
         </is>
       </c>
       <c r="B8" t="n">
-        <v>0</v>
+        <v>27.5</v>
       </c>
       <c r="C8" t="n">
-        <v>50.29</v>
+        <v>45.41</v>
       </c>
       <c r="D8" t="n">
         <v>1.24</v>
@@ -596,14 +596,14 @@
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>2025-12-15 22:05:05</t>
+          <t>2025-12-17 23:16:42</t>
         </is>
       </c>
       <c r="B9" t="n">
-        <v>0</v>
+        <v>27.5</v>
       </c>
       <c r="C9" t="n">
-        <v>50.29</v>
+        <v>45.41</v>
       </c>
       <c r="D9" t="n">
         <v>1.24</v>
@@ -615,14 +615,14 @@
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>2025-12-15 22:05:07</t>
+          <t>2025-12-17 23:16:43</t>
         </is>
       </c>
       <c r="B10" t="n">
-        <v>0</v>
+        <v>27.5</v>
       </c>
       <c r="C10" t="n">
-        <v>50.29</v>
+        <v>45.41</v>
       </c>
       <c r="D10" t="n">
         <v>1.24</v>
@@ -634,14 +634,14 @@
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>2025-12-15 22:05:08</t>
+          <t>2025-12-17 23:16:45</t>
         </is>
       </c>
       <c r="B11" t="n">
-        <v>0</v>
+        <v>27.5</v>
       </c>
       <c r="C11" t="n">
-        <v>50.29</v>
+        <v>45.41</v>
       </c>
       <c r="D11" t="n">
         <v>1.24</v>
@@ -653,14 +653,14 @@
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>2025-12-15 22:05:10</t>
+          <t>2025-12-17 23:16:46</t>
         </is>
       </c>
       <c r="B12" t="n">
-        <v>0</v>
+        <v>27.5</v>
       </c>
       <c r="C12" t="n">
-        <v>50.29</v>
+        <v>45.41</v>
       </c>
       <c r="D12" t="n">
         <v>1.24</v>
@@ -672,14 +672,14 @@
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>2025-12-15 22:05:11</t>
+          <t>2025-12-17 23:16:48</t>
         </is>
       </c>
       <c r="B13" t="n">
-        <v>0</v>
+        <v>27.5</v>
       </c>
       <c r="C13" t="n">
-        <v>50.29</v>
+        <v>45.41</v>
       </c>
       <c r="D13" t="n">
         <v>1.24</v>
@@ -691,14 +691,14 @@
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>2025-12-15 22:05:13</t>
+          <t>2025-12-17 23:16:49</t>
         </is>
       </c>
       <c r="B14" t="n">
-        <v>0</v>
+        <v>27.5</v>
       </c>
       <c r="C14" t="n">
-        <v>50.29</v>
+        <v>45.41</v>
       </c>
       <c r="D14" t="n">
         <v>1.24</v>
@@ -710,14 +710,14 @@
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>2025-12-15 22:05:15</t>
+          <t>2025-12-17 23:16:51</t>
         </is>
       </c>
       <c r="B15" t="n">
-        <v>0</v>
+        <v>27.5</v>
       </c>
       <c r="C15" t="n">
-        <v>50.29</v>
+        <v>45.41</v>
       </c>
       <c r="D15" t="n">
         <v>1.24</v>
@@ -729,14 +729,14 @@
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t>2025-12-15 22:05:17</t>
+          <t>2025-12-17 23:16:52</t>
         </is>
       </c>
       <c r="B16" t="n">
-        <v>0</v>
+        <v>27.5</v>
       </c>
       <c r="C16" t="n">
-        <v>50.29</v>
+        <v>45.41</v>
       </c>
       <c r="D16" t="n">
         <v>1.24</v>
@@ -748,19 +748,2147 @@
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
-          <t>2025-12-15 22:05:18</t>
+          <t>2025-12-17 23:16:54</t>
         </is>
       </c>
       <c r="B17" t="n">
-        <v>0</v>
+        <v>27.5</v>
       </c>
       <c r="C17" t="n">
-        <v>50.29</v>
+        <v>45.41</v>
       </c>
       <c r="D17" t="n">
         <v>1.24</v>
       </c>
       <c r="E17" t="n">
+        <v>2.7</v>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" t="inlineStr">
+        <is>
+          <t>2025-12-17 23:16:56</t>
+        </is>
+      </c>
+      <c r="B18" t="n">
+        <v>27.5</v>
+      </c>
+      <c r="C18" t="n">
+        <v>45.41</v>
+      </c>
+      <c r="D18" t="n">
+        <v>1.24</v>
+      </c>
+      <c r="E18" t="n">
+        <v>2.7</v>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" t="inlineStr">
+        <is>
+          <t>2025-12-17 23:16:58</t>
+        </is>
+      </c>
+      <c r="B19" t="n">
+        <v>27.5</v>
+      </c>
+      <c r="C19" t="n">
+        <v>45.41</v>
+      </c>
+      <c r="D19" t="n">
+        <v>1.24</v>
+      </c>
+      <c r="E19" t="n">
+        <v>2.7</v>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" t="inlineStr">
+        <is>
+          <t>2025-12-17 23:17:00</t>
+        </is>
+      </c>
+      <c r="B20" t="n">
+        <v>27.5</v>
+      </c>
+      <c r="C20" t="n">
+        <v>45.41</v>
+      </c>
+      <c r="D20" t="n">
+        <v>1.24</v>
+      </c>
+      <c r="E20" t="n">
+        <v>2.7</v>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" t="inlineStr">
+        <is>
+          <t>2025-12-17 23:17:01</t>
+        </is>
+      </c>
+      <c r="B21" t="n">
+        <v>27.5</v>
+      </c>
+      <c r="C21" t="n">
+        <v>45.41</v>
+      </c>
+      <c r="D21" t="n">
+        <v>1.24</v>
+      </c>
+      <c r="E21" t="n">
+        <v>2.7</v>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" t="inlineStr">
+        <is>
+          <t>2025-12-17 23:17:03</t>
+        </is>
+      </c>
+      <c r="B22" t="n">
+        <v>27.5</v>
+      </c>
+      <c r="C22" t="n">
+        <v>45.41</v>
+      </c>
+      <c r="D22" t="n">
+        <v>1.24</v>
+      </c>
+      <c r="E22" t="n">
+        <v>2.7</v>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" t="inlineStr">
+        <is>
+          <t>2025-12-17 23:17:04</t>
+        </is>
+      </c>
+      <c r="B23" t="n">
+        <v>27.5</v>
+      </c>
+      <c r="C23" t="n">
+        <v>45.41</v>
+      </c>
+      <c r="D23" t="n">
+        <v>1.24</v>
+      </c>
+      <c r="E23" t="n">
+        <v>2.7</v>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" t="inlineStr">
+        <is>
+          <t>2025-12-17 23:17:06</t>
+        </is>
+      </c>
+      <c r="B24" t="n">
+        <v>27.5</v>
+      </c>
+      <c r="C24" t="n">
+        <v>45.41</v>
+      </c>
+      <c r="D24" t="n">
+        <v>1.24</v>
+      </c>
+      <c r="E24" t="n">
+        <v>2.7</v>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25" t="inlineStr">
+        <is>
+          <t>2025-12-17 23:17:07</t>
+        </is>
+      </c>
+      <c r="B25" t="n">
+        <v>27.5</v>
+      </c>
+      <c r="C25" t="n">
+        <v>45.41</v>
+      </c>
+      <c r="D25" t="n">
+        <v>1.24</v>
+      </c>
+      <c r="E25" t="n">
+        <v>2.7</v>
+      </c>
+    </row>
+    <row r="26">
+      <c r="A26" t="inlineStr">
+        <is>
+          <t>2025-12-17 23:17:09</t>
+        </is>
+      </c>
+      <c r="B26" t="n">
+        <v>27.5</v>
+      </c>
+      <c r="C26" t="n">
+        <v>45.41</v>
+      </c>
+      <c r="D26" t="n">
+        <v>1.24</v>
+      </c>
+      <c r="E26" t="n">
+        <v>2.7</v>
+      </c>
+    </row>
+    <row r="27">
+      <c r="A27" t="inlineStr">
+        <is>
+          <t>2025-12-17 23:17:11</t>
+        </is>
+      </c>
+      <c r="B27" t="n">
+        <v>27.5</v>
+      </c>
+      <c r="C27" t="n">
+        <v>45.41</v>
+      </c>
+      <c r="D27" t="n">
+        <v>1.24</v>
+      </c>
+      <c r="E27" t="n">
+        <v>2.7</v>
+      </c>
+    </row>
+    <row r="28">
+      <c r="A28" t="inlineStr">
+        <is>
+          <t>2025-12-17 23:17:13</t>
+        </is>
+      </c>
+      <c r="B28" t="n">
+        <v>27.5</v>
+      </c>
+      <c r="C28" t="n">
+        <v>45.41</v>
+      </c>
+      <c r="D28" t="n">
+        <v>1.24</v>
+      </c>
+      <c r="E28" t="n">
+        <v>2.7</v>
+      </c>
+    </row>
+    <row r="29">
+      <c r="A29" t="inlineStr">
+        <is>
+          <t>2025-12-17 23:17:15</t>
+        </is>
+      </c>
+      <c r="B29" t="n">
+        <v>27.5</v>
+      </c>
+      <c r="C29" t="n">
+        <v>45.41</v>
+      </c>
+      <c r="D29" t="n">
+        <v>1.24</v>
+      </c>
+      <c r="E29" t="n">
+        <v>2.7</v>
+      </c>
+    </row>
+    <row r="30">
+      <c r="A30" t="inlineStr">
+        <is>
+          <t>2025-12-17 23:17:16</t>
+        </is>
+      </c>
+      <c r="B30" t="n">
+        <v>27.5</v>
+      </c>
+      <c r="C30" t="n">
+        <v>45.41</v>
+      </c>
+      <c r="D30" t="n">
+        <v>1.24</v>
+      </c>
+      <c r="E30" t="n">
+        <v>2.7</v>
+      </c>
+    </row>
+    <row r="31">
+      <c r="A31" t="inlineStr">
+        <is>
+          <t>2025-12-17 23:17:18</t>
+        </is>
+      </c>
+      <c r="B31" t="n">
+        <v>27.5</v>
+      </c>
+      <c r="C31" t="n">
+        <v>45.41</v>
+      </c>
+      <c r="D31" t="n">
+        <v>1.24</v>
+      </c>
+      <c r="E31" t="n">
+        <v>2.7</v>
+      </c>
+    </row>
+    <row r="32">
+      <c r="A32" t="inlineStr">
+        <is>
+          <t>2025-12-17 23:17:19</t>
+        </is>
+      </c>
+      <c r="B32" t="n">
+        <v>27.5</v>
+      </c>
+      <c r="C32" t="n">
+        <v>45.41</v>
+      </c>
+      <c r="D32" t="n">
+        <v>1.24</v>
+      </c>
+      <c r="E32" t="n">
+        <v>2.7</v>
+      </c>
+    </row>
+    <row r="33">
+      <c r="A33" t="inlineStr">
+        <is>
+          <t>2025-12-17 23:17:21</t>
+        </is>
+      </c>
+      <c r="B33" t="n">
+        <v>27.5</v>
+      </c>
+      <c r="C33" t="n">
+        <v>45.41</v>
+      </c>
+      <c r="D33" t="n">
+        <v>1.24</v>
+      </c>
+      <c r="E33" t="n">
+        <v>2.7</v>
+      </c>
+    </row>
+    <row r="34">
+      <c r="A34" t="inlineStr">
+        <is>
+          <t>2025-12-17 23:17:23</t>
+        </is>
+      </c>
+      <c r="B34" t="n">
+        <v>27.5</v>
+      </c>
+      <c r="C34" t="n">
+        <v>45.41</v>
+      </c>
+      <c r="D34" t="n">
+        <v>1.24</v>
+      </c>
+      <c r="E34" t="n">
+        <v>2.7</v>
+      </c>
+    </row>
+    <row r="35">
+      <c r="A35" t="inlineStr">
+        <is>
+          <t>2025-12-17 23:17:25</t>
+        </is>
+      </c>
+      <c r="B35" t="n">
+        <v>27.5</v>
+      </c>
+      <c r="C35" t="n">
+        <v>45.41</v>
+      </c>
+      <c r="D35" t="n">
+        <v>1.24</v>
+      </c>
+      <c r="E35" t="n">
+        <v>2.7</v>
+      </c>
+    </row>
+    <row r="36">
+      <c r="A36" t="inlineStr">
+        <is>
+          <t>2025-12-17 23:17:26</t>
+        </is>
+      </c>
+      <c r="B36" t="n">
+        <v>27.5</v>
+      </c>
+      <c r="C36" t="n">
+        <v>45.41</v>
+      </c>
+      <c r="D36" t="n">
+        <v>1.24</v>
+      </c>
+      <c r="E36" t="n">
+        <v>2.7</v>
+      </c>
+    </row>
+    <row r="37">
+      <c r="A37" t="inlineStr">
+        <is>
+          <t>2025-12-17 23:17:28</t>
+        </is>
+      </c>
+      <c r="B37" t="n">
+        <v>27.5</v>
+      </c>
+      <c r="C37" t="n">
+        <v>45.41</v>
+      </c>
+      <c r="D37" t="n">
+        <v>1.24</v>
+      </c>
+      <c r="E37" t="n">
+        <v>2.7</v>
+      </c>
+    </row>
+    <row r="38">
+      <c r="A38" t="inlineStr">
+        <is>
+          <t>2025-12-17 23:17:29</t>
+        </is>
+      </c>
+      <c r="B38" t="n">
+        <v>27.5</v>
+      </c>
+      <c r="C38" t="n">
+        <v>45.41</v>
+      </c>
+      <c r="D38" t="n">
+        <v>1.24</v>
+      </c>
+      <c r="E38" t="n">
+        <v>2.7</v>
+      </c>
+    </row>
+    <row r="39">
+      <c r="A39" t="inlineStr">
+        <is>
+          <t>2025-12-17 23:17:31</t>
+        </is>
+      </c>
+      <c r="B39" t="n">
+        <v>27.5</v>
+      </c>
+      <c r="C39" t="n">
+        <v>45.41</v>
+      </c>
+      <c r="D39" t="n">
+        <v>1.24</v>
+      </c>
+      <c r="E39" t="n">
+        <v>2.7</v>
+      </c>
+    </row>
+    <row r="40">
+      <c r="A40" t="inlineStr">
+        <is>
+          <t>2025-12-17 23:17:32</t>
+        </is>
+      </c>
+      <c r="B40" t="n">
+        <v>27.5</v>
+      </c>
+      <c r="C40" t="n">
+        <v>45.41</v>
+      </c>
+      <c r="D40" t="n">
+        <v>1.24</v>
+      </c>
+      <c r="E40" t="n">
+        <v>2.7</v>
+      </c>
+    </row>
+    <row r="41">
+      <c r="A41" t="inlineStr">
+        <is>
+          <t>2025-12-17 23:17:34</t>
+        </is>
+      </c>
+      <c r="B41" t="n">
+        <v>27.5</v>
+      </c>
+      <c r="C41" t="n">
+        <v>45.41</v>
+      </c>
+      <c r="D41" t="n">
+        <v>1.24</v>
+      </c>
+      <c r="E41" t="n">
+        <v>2.7</v>
+      </c>
+    </row>
+    <row r="42">
+      <c r="A42" t="inlineStr">
+        <is>
+          <t>2025-12-17 23:17:35</t>
+        </is>
+      </c>
+      <c r="B42" t="n">
+        <v>27.5</v>
+      </c>
+      <c r="C42" t="n">
+        <v>45.41</v>
+      </c>
+      <c r="D42" t="n">
+        <v>1.24</v>
+      </c>
+      <c r="E42" t="n">
+        <v>2.7</v>
+      </c>
+    </row>
+    <row r="43">
+      <c r="A43" t="inlineStr">
+        <is>
+          <t>2025-12-17 23:17:37</t>
+        </is>
+      </c>
+      <c r="B43" t="n">
+        <v>27.5</v>
+      </c>
+      <c r="C43" t="n">
+        <v>45.41</v>
+      </c>
+      <c r="D43" t="n">
+        <v>1.24</v>
+      </c>
+      <c r="E43" t="n">
+        <v>2.7</v>
+      </c>
+    </row>
+    <row r="44">
+      <c r="A44" t="inlineStr">
+        <is>
+          <t>2025-12-17 23:17:39</t>
+        </is>
+      </c>
+      <c r="B44" t="n">
+        <v>27.5</v>
+      </c>
+      <c r="C44" t="n">
+        <v>45.41</v>
+      </c>
+      <c r="D44" t="n">
+        <v>1.24</v>
+      </c>
+      <c r="E44" t="n">
+        <v>2.7</v>
+      </c>
+    </row>
+    <row r="45">
+      <c r="A45" t="inlineStr">
+        <is>
+          <t>2025-12-17 23:17:40</t>
+        </is>
+      </c>
+      <c r="B45" t="n">
+        <v>27.5</v>
+      </c>
+      <c r="C45" t="n">
+        <v>45.41</v>
+      </c>
+      <c r="D45" t="n">
+        <v>1.24</v>
+      </c>
+      <c r="E45" t="n">
+        <v>2.7</v>
+      </c>
+    </row>
+    <row r="46">
+      <c r="A46" t="inlineStr">
+        <is>
+          <t>2025-12-17 23:17:42</t>
+        </is>
+      </c>
+      <c r="B46" t="n">
+        <v>27.5</v>
+      </c>
+      <c r="C46" t="n">
+        <v>45.41</v>
+      </c>
+      <c r="D46" t="n">
+        <v>1.24</v>
+      </c>
+      <c r="E46" t="n">
+        <v>2.7</v>
+      </c>
+    </row>
+    <row r="47">
+      <c r="A47" t="inlineStr">
+        <is>
+          <t>2025-12-17 23:17:44</t>
+        </is>
+      </c>
+      <c r="B47" t="n">
+        <v>27.5</v>
+      </c>
+      <c r="C47" t="n">
+        <v>45.41</v>
+      </c>
+      <c r="D47" t="n">
+        <v>1.24</v>
+      </c>
+      <c r="E47" t="n">
+        <v>2.7</v>
+      </c>
+    </row>
+    <row r="48">
+      <c r="A48" t="inlineStr">
+        <is>
+          <t>2025-12-17 23:17:45</t>
+        </is>
+      </c>
+      <c r="B48" t="n">
+        <v>27.5</v>
+      </c>
+      <c r="C48" t="n">
+        <v>45.41</v>
+      </c>
+      <c r="D48" t="n">
+        <v>1.24</v>
+      </c>
+      <c r="E48" t="n">
+        <v>2.7</v>
+      </c>
+    </row>
+    <row r="49">
+      <c r="A49" t="inlineStr">
+        <is>
+          <t>2025-12-17 23:17:47</t>
+        </is>
+      </c>
+      <c r="B49" t="n">
+        <v>27.5</v>
+      </c>
+      <c r="C49" t="n">
+        <v>45.41</v>
+      </c>
+      <c r="D49" t="n">
+        <v>1.24</v>
+      </c>
+      <c r="E49" t="n">
+        <v>2.7</v>
+      </c>
+    </row>
+    <row r="50">
+      <c r="A50" t="inlineStr">
+        <is>
+          <t>2025-12-17 23:17:49</t>
+        </is>
+      </c>
+      <c r="B50" t="n">
+        <v>27.5</v>
+      </c>
+      <c r="C50" t="n">
+        <v>45.41</v>
+      </c>
+      <c r="D50" t="n">
+        <v>1.24</v>
+      </c>
+      <c r="E50" t="n">
+        <v>2.7</v>
+      </c>
+    </row>
+    <row r="51">
+      <c r="A51" t="inlineStr">
+        <is>
+          <t>2025-12-17 23:17:50</t>
+        </is>
+      </c>
+      <c r="B51" t="n">
+        <v>27.5</v>
+      </c>
+      <c r="C51" t="n">
+        <v>45.41</v>
+      </c>
+      <c r="D51" t="n">
+        <v>1.24</v>
+      </c>
+      <c r="E51" t="n">
+        <v>2.7</v>
+      </c>
+    </row>
+    <row r="52">
+      <c r="A52" t="inlineStr">
+        <is>
+          <t>2025-12-17 23:17:52</t>
+        </is>
+      </c>
+      <c r="B52" t="n">
+        <v>27.5</v>
+      </c>
+      <c r="C52" t="n">
+        <v>45.41</v>
+      </c>
+      <c r="D52" t="n">
+        <v>1.24</v>
+      </c>
+      <c r="E52" t="n">
+        <v>2.7</v>
+      </c>
+    </row>
+    <row r="53">
+      <c r="A53" t="inlineStr">
+        <is>
+          <t>2025-12-17 23:17:54</t>
+        </is>
+      </c>
+      <c r="B53" t="n">
+        <v>27.5</v>
+      </c>
+      <c r="C53" t="n">
+        <v>45.41</v>
+      </c>
+      <c r="D53" t="n">
+        <v>1.24</v>
+      </c>
+      <c r="E53" t="n">
+        <v>2.7</v>
+      </c>
+    </row>
+    <row r="54">
+      <c r="A54" t="inlineStr">
+        <is>
+          <t>2025-12-17 23:17:55</t>
+        </is>
+      </c>
+      <c r="B54" t="n">
+        <v>27.5</v>
+      </c>
+      <c r="C54" t="n">
+        <v>45.41</v>
+      </c>
+      <c r="D54" t="n">
+        <v>1.24</v>
+      </c>
+      <c r="E54" t="n">
+        <v>2.7</v>
+      </c>
+    </row>
+    <row r="55">
+      <c r="A55" t="inlineStr">
+        <is>
+          <t>2025-12-17 23:17:56</t>
+        </is>
+      </c>
+      <c r="B55" t="n">
+        <v>27.5</v>
+      </c>
+      <c r="C55" t="n">
+        <v>45.41</v>
+      </c>
+      <c r="D55" t="n">
+        <v>1.24</v>
+      </c>
+      <c r="E55" t="n">
+        <v>2.7</v>
+      </c>
+    </row>
+    <row r="56">
+      <c r="A56" t="inlineStr">
+        <is>
+          <t>2025-12-17 23:17:58</t>
+        </is>
+      </c>
+      <c r="B56" t="n">
+        <v>27.5</v>
+      </c>
+      <c r="C56" t="n">
+        <v>45.41</v>
+      </c>
+      <c r="D56" t="n">
+        <v>1.24</v>
+      </c>
+      <c r="E56" t="n">
+        <v>2.7</v>
+      </c>
+    </row>
+    <row r="57">
+      <c r="A57" t="inlineStr">
+        <is>
+          <t>2025-12-17 23:18:00</t>
+        </is>
+      </c>
+      <c r="B57" t="n">
+        <v>27.5</v>
+      </c>
+      <c r="C57" t="n">
+        <v>45.41</v>
+      </c>
+      <c r="D57" t="n">
+        <v>1.24</v>
+      </c>
+      <c r="E57" t="n">
+        <v>2.7</v>
+      </c>
+    </row>
+    <row r="58">
+      <c r="A58" t="inlineStr">
+        <is>
+          <t>2025-12-17 23:18:01</t>
+        </is>
+      </c>
+      <c r="B58" t="n">
+        <v>27.5</v>
+      </c>
+      <c r="C58" t="n">
+        <v>45.41</v>
+      </c>
+      <c r="D58" t="n">
+        <v>1.24</v>
+      </c>
+      <c r="E58" t="n">
+        <v>2.7</v>
+      </c>
+    </row>
+    <row r="59">
+      <c r="A59" t="inlineStr">
+        <is>
+          <t>2025-12-17 23:18:03</t>
+        </is>
+      </c>
+      <c r="B59" t="n">
+        <v>27.5</v>
+      </c>
+      <c r="C59" t="n">
+        <v>45.41</v>
+      </c>
+      <c r="D59" t="n">
+        <v>1.24</v>
+      </c>
+      <c r="E59" t="n">
+        <v>2.7</v>
+      </c>
+    </row>
+    <row r="60">
+      <c r="A60" t="inlineStr">
+        <is>
+          <t>2025-12-17 23:18:04</t>
+        </is>
+      </c>
+      <c r="B60" t="n">
+        <v>27.5</v>
+      </c>
+      <c r="C60" t="n">
+        <v>45.41</v>
+      </c>
+      <c r="D60" t="n">
+        <v>1.24</v>
+      </c>
+      <c r="E60" t="n">
+        <v>2.7</v>
+      </c>
+    </row>
+    <row r="61">
+      <c r="A61" t="inlineStr">
+        <is>
+          <t>2025-12-17 23:18:06</t>
+        </is>
+      </c>
+      <c r="B61" t="n">
+        <v>27.5</v>
+      </c>
+      <c r="C61" t="n">
+        <v>45.41</v>
+      </c>
+      <c r="D61" t="n">
+        <v>1.24</v>
+      </c>
+      <c r="E61" t="n">
+        <v>2.7</v>
+      </c>
+    </row>
+    <row r="62">
+      <c r="A62" t="inlineStr">
+        <is>
+          <t>2025-12-17 23:18:07</t>
+        </is>
+      </c>
+      <c r="B62" t="n">
+        <v>27.5</v>
+      </c>
+      <c r="C62" t="n">
+        <v>45.41</v>
+      </c>
+      <c r="D62" t="n">
+        <v>1.24</v>
+      </c>
+      <c r="E62" t="n">
+        <v>2.7</v>
+      </c>
+    </row>
+    <row r="63">
+      <c r="A63" t="inlineStr">
+        <is>
+          <t>2025-12-17 23:18:09</t>
+        </is>
+      </c>
+      <c r="B63" t="n">
+        <v>27.5</v>
+      </c>
+      <c r="C63" t="n">
+        <v>45.41</v>
+      </c>
+      <c r="D63" t="n">
+        <v>1.24</v>
+      </c>
+      <c r="E63" t="n">
+        <v>2.7</v>
+      </c>
+    </row>
+    <row r="64">
+      <c r="A64" t="inlineStr">
+        <is>
+          <t>2025-12-17 23:18:11</t>
+        </is>
+      </c>
+      <c r="B64" t="n">
+        <v>27.5</v>
+      </c>
+      <c r="C64" t="n">
+        <v>45.41</v>
+      </c>
+      <c r="D64" t="n">
+        <v>1.24</v>
+      </c>
+      <c r="E64" t="n">
+        <v>2.7</v>
+      </c>
+    </row>
+    <row r="65">
+      <c r="A65" t="inlineStr">
+        <is>
+          <t>2025-12-17 23:18:12</t>
+        </is>
+      </c>
+      <c r="B65" t="n">
+        <v>27.5</v>
+      </c>
+      <c r="C65" t="n">
+        <v>45.41</v>
+      </c>
+      <c r="D65" t="n">
+        <v>1.24</v>
+      </c>
+      <c r="E65" t="n">
+        <v>2.7</v>
+      </c>
+    </row>
+    <row r="66">
+      <c r="A66" t="inlineStr">
+        <is>
+          <t>2025-12-17 23:18:13</t>
+        </is>
+      </c>
+      <c r="B66" t="n">
+        <v>27.5</v>
+      </c>
+      <c r="C66" t="n">
+        <v>45.41</v>
+      </c>
+      <c r="D66" t="n">
+        <v>1.24</v>
+      </c>
+      <c r="E66" t="n">
+        <v>2.7</v>
+      </c>
+    </row>
+    <row r="67">
+      <c r="A67" t="inlineStr">
+        <is>
+          <t>2025-12-17 23:18:15</t>
+        </is>
+      </c>
+      <c r="B67" t="n">
+        <v>27.5</v>
+      </c>
+      <c r="C67" t="n">
+        <v>45.41</v>
+      </c>
+      <c r="D67" t="n">
+        <v>1.24</v>
+      </c>
+      <c r="E67" t="n">
+        <v>2.7</v>
+      </c>
+    </row>
+    <row r="68">
+      <c r="A68" t="inlineStr">
+        <is>
+          <t>2025-12-17 23:18:17</t>
+        </is>
+      </c>
+      <c r="B68" t="n">
+        <v>27.5</v>
+      </c>
+      <c r="C68" t="n">
+        <v>45.41</v>
+      </c>
+      <c r="D68" t="n">
+        <v>1.24</v>
+      </c>
+      <c r="E68" t="n">
+        <v>2.7</v>
+      </c>
+    </row>
+    <row r="69">
+      <c r="A69" t="inlineStr">
+        <is>
+          <t>2025-12-17 23:18:18</t>
+        </is>
+      </c>
+      <c r="B69" t="n">
+        <v>27.5</v>
+      </c>
+      <c r="C69" t="n">
+        <v>45.41</v>
+      </c>
+      <c r="D69" t="n">
+        <v>1.24</v>
+      </c>
+      <c r="E69" t="n">
+        <v>2.7</v>
+      </c>
+    </row>
+    <row r="70">
+      <c r="A70" t="inlineStr">
+        <is>
+          <t>2025-12-17 23:18:19</t>
+        </is>
+      </c>
+      <c r="B70" t="n">
+        <v>27.5</v>
+      </c>
+      <c r="C70" t="n">
+        <v>45.41</v>
+      </c>
+      <c r="D70" t="n">
+        <v>1.24</v>
+      </c>
+      <c r="E70" t="n">
+        <v>2.7</v>
+      </c>
+    </row>
+    <row r="71">
+      <c r="A71" t="inlineStr">
+        <is>
+          <t>2025-12-17 23:18:21</t>
+        </is>
+      </c>
+      <c r="B71" t="n">
+        <v>27.5</v>
+      </c>
+      <c r="C71" t="n">
+        <v>45.41</v>
+      </c>
+      <c r="D71" t="n">
+        <v>1.24</v>
+      </c>
+      <c r="E71" t="n">
+        <v>2.7</v>
+      </c>
+    </row>
+    <row r="72">
+      <c r="A72" t="inlineStr">
+        <is>
+          <t>2025-12-17 23:18:22</t>
+        </is>
+      </c>
+      <c r="B72" t="n">
+        <v>27.5</v>
+      </c>
+      <c r="C72" t="n">
+        <v>45.41</v>
+      </c>
+      <c r="D72" t="n">
+        <v>1.24</v>
+      </c>
+      <c r="E72" t="n">
+        <v>2.7</v>
+      </c>
+    </row>
+    <row r="73">
+      <c r="A73" t="inlineStr">
+        <is>
+          <t>2025-12-17 23:18:24</t>
+        </is>
+      </c>
+      <c r="B73" t="n">
+        <v>27.5</v>
+      </c>
+      <c r="C73" t="n">
+        <v>45.41</v>
+      </c>
+      <c r="D73" t="n">
+        <v>1.24</v>
+      </c>
+      <c r="E73" t="n">
+        <v>2.7</v>
+      </c>
+    </row>
+    <row r="74">
+      <c r="A74" t="inlineStr">
+        <is>
+          <t>2025-12-17 23:18:25</t>
+        </is>
+      </c>
+      <c r="B74" t="n">
+        <v>27.5</v>
+      </c>
+      <c r="C74" t="n">
+        <v>45.41</v>
+      </c>
+      <c r="D74" t="n">
+        <v>1.24</v>
+      </c>
+      <c r="E74" t="n">
+        <v>2.7</v>
+      </c>
+    </row>
+    <row r="75">
+      <c r="A75" t="inlineStr">
+        <is>
+          <t>2025-12-17 23:18:27</t>
+        </is>
+      </c>
+      <c r="B75" t="n">
+        <v>27.5</v>
+      </c>
+      <c r="C75" t="n">
+        <v>45.41</v>
+      </c>
+      <c r="D75" t="n">
+        <v>1.24</v>
+      </c>
+      <c r="E75" t="n">
+        <v>2.7</v>
+      </c>
+    </row>
+    <row r="76">
+      <c r="A76" t="inlineStr">
+        <is>
+          <t>2025-12-17 23:18:28</t>
+        </is>
+      </c>
+      <c r="B76" t="n">
+        <v>27.5</v>
+      </c>
+      <c r="C76" t="n">
+        <v>45.41</v>
+      </c>
+      <c r="D76" t="n">
+        <v>1.24</v>
+      </c>
+      <c r="E76" t="n">
+        <v>2.7</v>
+      </c>
+    </row>
+    <row r="77">
+      <c r="A77" t="inlineStr">
+        <is>
+          <t>2025-12-17 23:18:30</t>
+        </is>
+      </c>
+      <c r="B77" t="n">
+        <v>27.5</v>
+      </c>
+      <c r="C77" t="n">
+        <v>45.41</v>
+      </c>
+      <c r="D77" t="n">
+        <v>1.24</v>
+      </c>
+      <c r="E77" t="n">
+        <v>2.7</v>
+      </c>
+    </row>
+    <row r="78">
+      <c r="A78" t="inlineStr">
+        <is>
+          <t>2025-12-17 23:18:31</t>
+        </is>
+      </c>
+      <c r="B78" t="n">
+        <v>27.5</v>
+      </c>
+      <c r="C78" t="n">
+        <v>45.41</v>
+      </c>
+      <c r="D78" t="n">
+        <v>1.24</v>
+      </c>
+      <c r="E78" t="n">
+        <v>2.7</v>
+      </c>
+    </row>
+    <row r="79">
+      <c r="A79" t="inlineStr">
+        <is>
+          <t>2025-12-17 23:18:33</t>
+        </is>
+      </c>
+      <c r="B79" t="n">
+        <v>27.5</v>
+      </c>
+      <c r="C79" t="n">
+        <v>45.41</v>
+      </c>
+      <c r="D79" t="n">
+        <v>1.24</v>
+      </c>
+      <c r="E79" t="n">
+        <v>2.7</v>
+      </c>
+    </row>
+    <row r="80">
+      <c r="A80" t="inlineStr">
+        <is>
+          <t>2025-12-17 23:18:34</t>
+        </is>
+      </c>
+      <c r="B80" t="n">
+        <v>27.5</v>
+      </c>
+      <c r="C80" t="n">
+        <v>45.41</v>
+      </c>
+      <c r="D80" t="n">
+        <v>1.24</v>
+      </c>
+      <c r="E80" t="n">
+        <v>2.7</v>
+      </c>
+    </row>
+    <row r="81">
+      <c r="A81" t="inlineStr">
+        <is>
+          <t>2025-12-17 23:18:36</t>
+        </is>
+      </c>
+      <c r="B81" t="n">
+        <v>27.5</v>
+      </c>
+      <c r="C81" t="n">
+        <v>45.41</v>
+      </c>
+      <c r="D81" t="n">
+        <v>1.24</v>
+      </c>
+      <c r="E81" t="n">
+        <v>2.7</v>
+      </c>
+    </row>
+    <row r="82">
+      <c r="A82" t="inlineStr">
+        <is>
+          <t>2025-12-17 23:18:38</t>
+        </is>
+      </c>
+      <c r="B82" t="n">
+        <v>27.5</v>
+      </c>
+      <c r="C82" t="n">
+        <v>45.41</v>
+      </c>
+      <c r="D82" t="n">
+        <v>1.24</v>
+      </c>
+      <c r="E82" t="n">
+        <v>2.7</v>
+      </c>
+    </row>
+    <row r="83">
+      <c r="A83" t="inlineStr">
+        <is>
+          <t>2025-12-17 23:18:39</t>
+        </is>
+      </c>
+      <c r="B83" t="n">
+        <v>27.5</v>
+      </c>
+      <c r="C83" t="n">
+        <v>45.41</v>
+      </c>
+      <c r="D83" t="n">
+        <v>1.24</v>
+      </c>
+      <c r="E83" t="n">
+        <v>2.7</v>
+      </c>
+    </row>
+    <row r="84">
+      <c r="A84" t="inlineStr">
+        <is>
+          <t>2025-12-17 23:18:42</t>
+        </is>
+      </c>
+      <c r="B84" t="n">
+        <v>27.5</v>
+      </c>
+      <c r="C84" t="n">
+        <v>45.41</v>
+      </c>
+      <c r="D84" t="n">
+        <v>1.24</v>
+      </c>
+      <c r="E84" t="n">
+        <v>2.7</v>
+      </c>
+    </row>
+    <row r="85">
+      <c r="A85" t="inlineStr">
+        <is>
+          <t>2025-12-17 23:18:44</t>
+        </is>
+      </c>
+      <c r="B85" t="n">
+        <v>27.5</v>
+      </c>
+      <c r="C85" t="n">
+        <v>45.41</v>
+      </c>
+      <c r="D85" t="n">
+        <v>1.24</v>
+      </c>
+      <c r="E85" t="n">
+        <v>2.7</v>
+      </c>
+    </row>
+    <row r="86">
+      <c r="A86" t="inlineStr">
+        <is>
+          <t>2025-12-17 23:18:45</t>
+        </is>
+      </c>
+      <c r="B86" t="n">
+        <v>27.5</v>
+      </c>
+      <c r="C86" t="n">
+        <v>45.41</v>
+      </c>
+      <c r="D86" t="n">
+        <v>1.24</v>
+      </c>
+      <c r="E86" t="n">
+        <v>2.7</v>
+      </c>
+    </row>
+    <row r="87">
+      <c r="A87" t="inlineStr">
+        <is>
+          <t>2025-12-17 23:18:47</t>
+        </is>
+      </c>
+      <c r="B87" t="n">
+        <v>27.5</v>
+      </c>
+      <c r="C87" t="n">
+        <v>45.41</v>
+      </c>
+      <c r="D87" t="n">
+        <v>1.24</v>
+      </c>
+      <c r="E87" t="n">
+        <v>2.7</v>
+      </c>
+    </row>
+    <row r="88">
+      <c r="A88" t="inlineStr">
+        <is>
+          <t>2025-12-17 23:18:48</t>
+        </is>
+      </c>
+      <c r="B88" t="n">
+        <v>27.5</v>
+      </c>
+      <c r="C88" t="n">
+        <v>45.41</v>
+      </c>
+      <c r="D88" t="n">
+        <v>1.24</v>
+      </c>
+      <c r="E88" t="n">
+        <v>2.7</v>
+      </c>
+    </row>
+    <row r="89">
+      <c r="A89" t="inlineStr">
+        <is>
+          <t>2025-12-17 23:18:50</t>
+        </is>
+      </c>
+      <c r="B89" t="n">
+        <v>27.5</v>
+      </c>
+      <c r="C89" t="n">
+        <v>45.41</v>
+      </c>
+      <c r="D89" t="n">
+        <v>1.24</v>
+      </c>
+      <c r="E89" t="n">
+        <v>2.7</v>
+      </c>
+    </row>
+    <row r="90">
+      <c r="A90" t="inlineStr">
+        <is>
+          <t>2025-12-17 23:18:52</t>
+        </is>
+      </c>
+      <c r="B90" t="n">
+        <v>27.5</v>
+      </c>
+      <c r="C90" t="n">
+        <v>45.41</v>
+      </c>
+      <c r="D90" t="n">
+        <v>1.24</v>
+      </c>
+      <c r="E90" t="n">
+        <v>2.7</v>
+      </c>
+    </row>
+    <row r="91">
+      <c r="A91" t="inlineStr">
+        <is>
+          <t>2025-12-17 23:18:53</t>
+        </is>
+      </c>
+      <c r="B91" t="n">
+        <v>27.5</v>
+      </c>
+      <c r="C91" t="n">
+        <v>45.41</v>
+      </c>
+      <c r="D91" t="n">
+        <v>1.24</v>
+      </c>
+      <c r="E91" t="n">
+        <v>2.7</v>
+      </c>
+    </row>
+    <row r="92">
+      <c r="A92" t="inlineStr">
+        <is>
+          <t>2025-12-17 23:18:56</t>
+        </is>
+      </c>
+      <c r="B92" t="n">
+        <v>27.5</v>
+      </c>
+      <c r="C92" t="n">
+        <v>45.41</v>
+      </c>
+      <c r="D92" t="n">
+        <v>1.24</v>
+      </c>
+      <c r="E92" t="n">
+        <v>2.7</v>
+      </c>
+    </row>
+    <row r="93">
+      <c r="A93" t="inlineStr">
+        <is>
+          <t>2025-12-17 23:18:57</t>
+        </is>
+      </c>
+      <c r="B93" t="n">
+        <v>27.5</v>
+      </c>
+      <c r="C93" t="n">
+        <v>45.41</v>
+      </c>
+      <c r="D93" t="n">
+        <v>1.24</v>
+      </c>
+      <c r="E93" t="n">
+        <v>2.7</v>
+      </c>
+    </row>
+    <row r="94">
+      <c r="A94" t="inlineStr">
+        <is>
+          <t>2025-12-17 23:18:59</t>
+        </is>
+      </c>
+      <c r="B94" t="n">
+        <v>27.5</v>
+      </c>
+      <c r="C94" t="n">
+        <v>45.41</v>
+      </c>
+      <c r="D94" t="n">
+        <v>1.24</v>
+      </c>
+      <c r="E94" t="n">
+        <v>2.7</v>
+      </c>
+    </row>
+    <row r="95">
+      <c r="A95" t="inlineStr">
+        <is>
+          <t>2025-12-17 23:19:01</t>
+        </is>
+      </c>
+      <c r="B95" t="n">
+        <v>27.5</v>
+      </c>
+      <c r="C95" t="n">
+        <v>45.41</v>
+      </c>
+      <c r="D95" t="n">
+        <v>1.24</v>
+      </c>
+      <c r="E95" t="n">
+        <v>2.7</v>
+      </c>
+    </row>
+    <row r="96">
+      <c r="A96" t="inlineStr">
+        <is>
+          <t>2025-12-17 23:19:02</t>
+        </is>
+      </c>
+      <c r="B96" t="n">
+        <v>27.5</v>
+      </c>
+      <c r="C96" t="n">
+        <v>45.41</v>
+      </c>
+      <c r="D96" t="n">
+        <v>1.24</v>
+      </c>
+      <c r="E96" t="n">
+        <v>2.7</v>
+      </c>
+    </row>
+    <row r="97">
+      <c r="A97" t="inlineStr">
+        <is>
+          <t>2025-12-17 23:19:05</t>
+        </is>
+      </c>
+      <c r="B97" t="n">
+        <v>27.5</v>
+      </c>
+      <c r="C97" t="n">
+        <v>45.41</v>
+      </c>
+      <c r="D97" t="n">
+        <v>1.24</v>
+      </c>
+      <c r="E97" t="n">
+        <v>2.7</v>
+      </c>
+    </row>
+    <row r="98">
+      <c r="A98" t="inlineStr">
+        <is>
+          <t>2025-12-17 23:19:06</t>
+        </is>
+      </c>
+      <c r="B98" t="n">
+        <v>27.5</v>
+      </c>
+      <c r="C98" t="n">
+        <v>45.41</v>
+      </c>
+      <c r="D98" t="n">
+        <v>1.24</v>
+      </c>
+      <c r="E98" t="n">
+        <v>2.7</v>
+      </c>
+    </row>
+    <row r="99">
+      <c r="A99" t="inlineStr">
+        <is>
+          <t>2025-12-17 23:19:08</t>
+        </is>
+      </c>
+      <c r="B99" t="n">
+        <v>27.5</v>
+      </c>
+      <c r="C99" t="n">
+        <v>45.41</v>
+      </c>
+      <c r="D99" t="n">
+        <v>1.24</v>
+      </c>
+      <c r="E99" t="n">
+        <v>2.7</v>
+      </c>
+    </row>
+    <row r="100">
+      <c r="A100" t="inlineStr">
+        <is>
+          <t>2025-12-17 23:19:10</t>
+        </is>
+      </c>
+      <c r="B100" t="n">
+        <v>27.5</v>
+      </c>
+      <c r="C100" t="n">
+        <v>45.41</v>
+      </c>
+      <c r="D100" t="n">
+        <v>1.24</v>
+      </c>
+      <c r="E100" t="n">
+        <v>2.7</v>
+      </c>
+    </row>
+    <row r="101">
+      <c r="A101" t="inlineStr">
+        <is>
+          <t>2025-12-17 23:19:12</t>
+        </is>
+      </c>
+      <c r="B101" t="n">
+        <v>27.5</v>
+      </c>
+      <c r="C101" t="n">
+        <v>45.41</v>
+      </c>
+      <c r="D101" t="n">
+        <v>1.24</v>
+      </c>
+      <c r="E101" t="n">
+        <v>2.7</v>
+      </c>
+    </row>
+    <row r="102">
+      <c r="A102" t="inlineStr">
+        <is>
+          <t>2025-12-17 23:19:14</t>
+        </is>
+      </c>
+      <c r="B102" t="n">
+        <v>27.5</v>
+      </c>
+      <c r="C102" t="n">
+        <v>45.41</v>
+      </c>
+      <c r="D102" t="n">
+        <v>1.24</v>
+      </c>
+      <c r="E102" t="n">
+        <v>2.7</v>
+      </c>
+    </row>
+    <row r="103">
+      <c r="A103" t="inlineStr">
+        <is>
+          <t>2025-12-17 23:19:15</t>
+        </is>
+      </c>
+      <c r="B103" t="n">
+        <v>27.5</v>
+      </c>
+      <c r="C103" t="n">
+        <v>45.41</v>
+      </c>
+      <c r="D103" t="n">
+        <v>1.24</v>
+      </c>
+      <c r="E103" t="n">
+        <v>2.7</v>
+      </c>
+    </row>
+    <row r="104">
+      <c r="A104" t="inlineStr">
+        <is>
+          <t>2025-12-17 23:19:17</t>
+        </is>
+      </c>
+      <c r="B104" t="n">
+        <v>27.5</v>
+      </c>
+      <c r="C104" t="n">
+        <v>45.41</v>
+      </c>
+      <c r="D104" t="n">
+        <v>1.24</v>
+      </c>
+      <c r="E104" t="n">
+        <v>2.7</v>
+      </c>
+    </row>
+    <row r="105">
+      <c r="A105" t="inlineStr">
+        <is>
+          <t>2025-12-17 23:19:19</t>
+        </is>
+      </c>
+      <c r="B105" t="n">
+        <v>27.5</v>
+      </c>
+      <c r="C105" t="n">
+        <v>45.41</v>
+      </c>
+      <c r="D105" t="n">
+        <v>1.24</v>
+      </c>
+      <c r="E105" t="n">
+        <v>2.7</v>
+      </c>
+    </row>
+    <row r="106">
+      <c r="A106" t="inlineStr">
+        <is>
+          <t>2025-12-17 23:19:21</t>
+        </is>
+      </c>
+      <c r="B106" t="n">
+        <v>27.5</v>
+      </c>
+      <c r="C106" t="n">
+        <v>45.41</v>
+      </c>
+      <c r="D106" t="n">
+        <v>1.24</v>
+      </c>
+      <c r="E106" t="n">
+        <v>2.7</v>
+      </c>
+    </row>
+    <row r="107">
+      <c r="A107" t="inlineStr">
+        <is>
+          <t>2025-12-17 23:19:22</t>
+        </is>
+      </c>
+      <c r="B107" t="n">
+        <v>27.5</v>
+      </c>
+      <c r="C107" t="n">
+        <v>45.41</v>
+      </c>
+      <c r="D107" t="n">
+        <v>1.24</v>
+      </c>
+      <c r="E107" t="n">
+        <v>2.7</v>
+      </c>
+    </row>
+    <row r="108">
+      <c r="A108" t="inlineStr">
+        <is>
+          <t>2025-12-17 23:19:24</t>
+        </is>
+      </c>
+      <c r="B108" t="n">
+        <v>27.5</v>
+      </c>
+      <c r="C108" t="n">
+        <v>45.41</v>
+      </c>
+      <c r="D108" t="n">
+        <v>1.24</v>
+      </c>
+      <c r="E108" t="n">
+        <v>2.7</v>
+      </c>
+    </row>
+    <row r="109">
+      <c r="A109" t="inlineStr">
+        <is>
+          <t>2025-12-17 23:19:26</t>
+        </is>
+      </c>
+      <c r="B109" t="n">
+        <v>27.5</v>
+      </c>
+      <c r="C109" t="n">
+        <v>45.41</v>
+      </c>
+      <c r="D109" t="n">
+        <v>1.24</v>
+      </c>
+      <c r="E109" t="n">
+        <v>2.7</v>
+      </c>
+    </row>
+    <row r="110">
+      <c r="A110" t="inlineStr">
+        <is>
+          <t>2025-12-17 23:19:27</t>
+        </is>
+      </c>
+      <c r="B110" t="n">
+        <v>27.5</v>
+      </c>
+      <c r="C110" t="n">
+        <v>45.41</v>
+      </c>
+      <c r="D110" t="n">
+        <v>1.24</v>
+      </c>
+      <c r="E110" t="n">
+        <v>2.7</v>
+      </c>
+    </row>
+    <row r="111">
+      <c r="A111" t="inlineStr">
+        <is>
+          <t>2025-12-17 23:19:29</t>
+        </is>
+      </c>
+      <c r="B111" t="n">
+        <v>27.5</v>
+      </c>
+      <c r="C111" t="n">
+        <v>45.41</v>
+      </c>
+      <c r="D111" t="n">
+        <v>1.24</v>
+      </c>
+      <c r="E111" t="n">
+        <v>2.7</v>
+      </c>
+    </row>
+    <row r="112">
+      <c r="A112" t="inlineStr">
+        <is>
+          <t>2025-12-17 23:19:30</t>
+        </is>
+      </c>
+      <c r="B112" t="n">
+        <v>27.5</v>
+      </c>
+      <c r="C112" t="n">
+        <v>45.41</v>
+      </c>
+      <c r="D112" t="n">
+        <v>1.24</v>
+      </c>
+      <c r="E112" t="n">
+        <v>2.7</v>
+      </c>
+    </row>
+    <row r="113">
+      <c r="A113" t="inlineStr">
+        <is>
+          <t>2025-12-17 23:19:32</t>
+        </is>
+      </c>
+      <c r="B113" t="n">
+        <v>27.5</v>
+      </c>
+      <c r="C113" t="n">
+        <v>45.41</v>
+      </c>
+      <c r="D113" t="n">
+        <v>1.24</v>
+      </c>
+      <c r="E113" t="n">
+        <v>2.7</v>
+      </c>
+    </row>
+    <row r="114">
+      <c r="A114" t="inlineStr">
+        <is>
+          <t>2025-12-17 23:19:33</t>
+        </is>
+      </c>
+      <c r="B114" t="n">
+        <v>27.5</v>
+      </c>
+      <c r="C114" t="n">
+        <v>45.41</v>
+      </c>
+      <c r="D114" t="n">
+        <v>1.24</v>
+      </c>
+      <c r="E114" t="n">
+        <v>2.7</v>
+      </c>
+    </row>
+    <row r="115">
+      <c r="A115" t="inlineStr">
+        <is>
+          <t>2025-12-17 23:19:34</t>
+        </is>
+      </c>
+      <c r="B115" t="n">
+        <v>27.5</v>
+      </c>
+      <c r="C115" t="n">
+        <v>45.41</v>
+      </c>
+      <c r="D115" t="n">
+        <v>1.24</v>
+      </c>
+      <c r="E115" t="n">
+        <v>2.7</v>
+      </c>
+    </row>
+    <row r="116">
+      <c r="A116" t="inlineStr">
+        <is>
+          <t>2025-12-17 23:19:36</t>
+        </is>
+      </c>
+      <c r="B116" t="n">
+        <v>27.5</v>
+      </c>
+      <c r="C116" t="n">
+        <v>45.41</v>
+      </c>
+      <c r="D116" t="n">
+        <v>1.24</v>
+      </c>
+      <c r="E116" t="n">
+        <v>2.7</v>
+      </c>
+    </row>
+    <row r="117">
+      <c r="A117" t="inlineStr">
+        <is>
+          <t>2025-12-17 23:19:37</t>
+        </is>
+      </c>
+      <c r="B117" t="n">
+        <v>27.5</v>
+      </c>
+      <c r="C117" t="n">
+        <v>45.41</v>
+      </c>
+      <c r="D117" t="n">
+        <v>1.24</v>
+      </c>
+      <c r="E117" t="n">
+        <v>2.7</v>
+      </c>
+    </row>
+    <row r="118">
+      <c r="A118" t="inlineStr">
+        <is>
+          <t>2025-12-17 23:19:39</t>
+        </is>
+      </c>
+      <c r="B118" t="n">
+        <v>27.5</v>
+      </c>
+      <c r="C118" t="n">
+        <v>45.41</v>
+      </c>
+      <c r="D118" t="n">
+        <v>1.24</v>
+      </c>
+      <c r="E118" t="n">
+        <v>2.7</v>
+      </c>
+    </row>
+    <row r="119">
+      <c r="A119" t="inlineStr">
+        <is>
+          <t>2025-12-17 23:19:41</t>
+        </is>
+      </c>
+      <c r="B119" t="n">
+        <v>27.5</v>
+      </c>
+      <c r="C119" t="n">
+        <v>45.41</v>
+      </c>
+      <c r="D119" t="n">
+        <v>1.24</v>
+      </c>
+      <c r="E119" t="n">
+        <v>2.7</v>
+      </c>
+    </row>
+    <row r="120">
+      <c r="A120" t="inlineStr">
+        <is>
+          <t>2025-12-17 23:19:42</t>
+        </is>
+      </c>
+      <c r="B120" t="n">
+        <v>27.5</v>
+      </c>
+      <c r="C120" t="n">
+        <v>45.41</v>
+      </c>
+      <c r="D120" t="n">
+        <v>1.24</v>
+      </c>
+      <c r="E120" t="n">
+        <v>2.7</v>
+      </c>
+    </row>
+    <row r="121">
+      <c r="A121" t="inlineStr">
+        <is>
+          <t>2025-12-17 23:19:44</t>
+        </is>
+      </c>
+      <c r="B121" t="n">
+        <v>27.5</v>
+      </c>
+      <c r="C121" t="n">
+        <v>45.41</v>
+      </c>
+      <c r="D121" t="n">
+        <v>1.24</v>
+      </c>
+      <c r="E121" t="n">
+        <v>2.7</v>
+      </c>
+    </row>
+    <row r="122">
+      <c r="A122" t="inlineStr">
+        <is>
+          <t>2025-12-17 23:19:45</t>
+        </is>
+      </c>
+      <c r="B122" t="n">
+        <v>27.5</v>
+      </c>
+      <c r="C122" t="n">
+        <v>45.41</v>
+      </c>
+      <c r="D122" t="n">
+        <v>1.24</v>
+      </c>
+      <c r="E122" t="n">
+        <v>2.7</v>
+      </c>
+    </row>
+    <row r="123">
+      <c r="A123" t="inlineStr">
+        <is>
+          <t>2025-12-17 23:19:47</t>
+        </is>
+      </c>
+      <c r="B123" t="n">
+        <v>27.5</v>
+      </c>
+      <c r="C123" t="n">
+        <v>45.41</v>
+      </c>
+      <c r="D123" t="n">
+        <v>1.24</v>
+      </c>
+      <c r="E123" t="n">
+        <v>2.7</v>
+      </c>
+    </row>
+    <row r="124">
+      <c r="A124" t="inlineStr">
+        <is>
+          <t>2025-12-17 23:19:48</t>
+        </is>
+      </c>
+      <c r="B124" t="n">
+        <v>27.5</v>
+      </c>
+      <c r="C124" t="n">
+        <v>45.41</v>
+      </c>
+      <c r="D124" t="n">
+        <v>1.24</v>
+      </c>
+      <c r="E124" t="n">
+        <v>2.7</v>
+      </c>
+    </row>
+    <row r="125">
+      <c r="A125" t="inlineStr">
+        <is>
+          <t>2025-12-17 23:19:50</t>
+        </is>
+      </c>
+      <c r="B125" t="n">
+        <v>27.5</v>
+      </c>
+      <c r="C125" t="n">
+        <v>45.41</v>
+      </c>
+      <c r="D125" t="n">
+        <v>1.24</v>
+      </c>
+      <c r="E125" t="n">
+        <v>2.7</v>
+      </c>
+    </row>
+    <row r="126">
+      <c r="A126" t="inlineStr">
+        <is>
+          <t>2025-12-17 23:19:51</t>
+        </is>
+      </c>
+      <c r="B126" t="n">
+        <v>27.5</v>
+      </c>
+      <c r="C126" t="n">
+        <v>45.41</v>
+      </c>
+      <c r="D126" t="n">
+        <v>1.24</v>
+      </c>
+      <c r="E126" t="n">
+        <v>2.7</v>
+      </c>
+    </row>
+    <row r="127">
+      <c r="A127" t="inlineStr">
+        <is>
+          <t>2025-12-17 23:19:53</t>
+        </is>
+      </c>
+      <c r="B127" t="n">
+        <v>27.5</v>
+      </c>
+      <c r="C127" t="n">
+        <v>45.41</v>
+      </c>
+      <c r="D127" t="n">
+        <v>1.24</v>
+      </c>
+      <c r="E127" t="n">
+        <v>2.7</v>
+      </c>
+    </row>
+    <row r="128">
+      <c r="A128" t="inlineStr">
+        <is>
+          <t>2025-12-17 23:19:54</t>
+        </is>
+      </c>
+      <c r="B128" t="n">
+        <v>27.5</v>
+      </c>
+      <c r="C128" t="n">
+        <v>45.41</v>
+      </c>
+      <c r="D128" t="n">
+        <v>1.24</v>
+      </c>
+      <c r="E128" t="n">
+        <v>2.7</v>
+      </c>
+    </row>
+    <row r="129">
+      <c r="A129" t="inlineStr">
+        <is>
+          <t>2025-12-17 23:19:56</t>
+        </is>
+      </c>
+      <c r="B129" t="n">
+        <v>27.5</v>
+      </c>
+      <c r="C129" t="n">
+        <v>45.41</v>
+      </c>
+      <c r="D129" t="n">
+        <v>1.24</v>
+      </c>
+      <c r="E129" t="n">
         <v>2.7</v>
       </c>
     </row>

</xml_diff>